<commit_message>
change scalar and vector index engine to btree in btree table
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/btreecases/dql/casegroup1/sql_dql_cases1_btree.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/btreecases/dql/casegroup1/sql_dql_cases1_btree.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15584" uniqueCount="5964">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15594" uniqueCount="5970">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -21014,6 +21014,28 @@
   </si>
   <si>
     <t>src/test/resources/io.dingodb.test/testdata/btreecases/dql/casegroup1/expectedresult/ComplexDataType/array/btree_queryc1_1793.csv</t>
+  </si>
+  <si>
+    <t>dqlc1_1794</t>
+  </si>
+  <si>
+    <t>float array字段在中间，通过array后字段条件仅查询array字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComplexDataType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select user_data from $array23 where amount&lt;1000 and age&lt;10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/btreecases/dql/casegroup1/expectedresult/ComplexDataType/array/btree_queryc1_1794.csv</t>
   </si>
 </sst>
 </file>
@@ -21394,10 +21416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1794"/>
+  <dimension ref="A1:K1795"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1765" workbookViewId="0">
-      <selection activeCell="C1800" sqref="C1800"/>
+    <sheetView tabSelected="1" topLeftCell="G1765" workbookViewId="0">
+      <selection activeCell="K1798" sqref="K1798"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -71771,6 +71793,39 @@
         <v>5963</v>
       </c>
       <c r="K1794" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1795" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1795" s="12" t="s">
+        <v>5964</v>
+      </c>
+      <c r="B1795" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1795" s="12" t="s">
+        <v>5965</v>
+      </c>
+      <c r="D1795" s="12" t="s">
+        <v>5966</v>
+      </c>
+      <c r="E1795" s="12" t="s">
+        <v>5967</v>
+      </c>
+      <c r="F1795" s="12" t="s">
+        <v>5953</v>
+      </c>
+      <c r="G1795" s="12"/>
+      <c r="H1795" s="12" t="s">
+        <v>5959</v>
+      </c>
+      <c r="I1795" s="12" t="s">
+        <v>5968</v>
+      </c>
+      <c r="J1795" s="12" t="s">
+        <v>5969</v>
+      </c>
+      <c r="K1795" s="12" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add txn_btree cases but disabled at present
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/btreecases/dql/casegroup1/sql_dql_cases1_btree.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/btreecases/dql/casegroup1/sql_dql_cases1_btree.xlsx
@@ -21016,9 +21016,6 @@
     <t>src/test/resources/io.dingodb.test/testdata/btreecases/dql/casegroup1/expectedresult/ComplexDataType/array/btree_queryc1_1793.csv</t>
   </si>
   <si>
-    <t>dqlc1_1794</t>
-  </si>
-  <si>
     <t>float array字段在中间，通过array后字段条件仅查询array字段</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -21036,6 +21033,9 @@
   </si>
   <si>
     <t>src/test/resources/io.dingodb.test/testdata/btreecases/dql/casegroup1/expectedresult/ComplexDataType/array/btree_queryc1_1794.csv</t>
+  </si>
+  <si>
+    <t>btree_dqlc1_1794</t>
   </si>
 </sst>
 </file>
@@ -21418,8 +21418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1795"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1765" workbookViewId="0">
-      <selection activeCell="K1798" sqref="K1798"/>
+    <sheetView tabSelected="1" topLeftCell="A1765" workbookViewId="0">
+      <selection activeCell="C1798" sqref="C1798"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -71702,7 +71702,7 @@
         <v>5958</v>
       </c>
       <c r="B1792" s="12" t="s">
-        <v>34</v>
+        <v>2906</v>
       </c>
       <c r="C1792" s="12" t="s">
         <v>5946</v>
@@ -71735,7 +71735,7 @@
         <v>5959</v>
       </c>
       <c r="B1793" s="12" t="s">
-        <v>34</v>
+        <v>2906</v>
       </c>
       <c r="C1793" s="12" t="s">
         <v>5952</v>
@@ -71768,7 +71768,7 @@
         <v>5960</v>
       </c>
       <c r="B1794" s="12" t="s">
-        <v>34</v>
+        <v>2906</v>
       </c>
       <c r="C1794" s="12" t="s">
         <v>5956</v>
@@ -71798,19 +71798,19 @@
     </row>
     <row r="1795" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1795" s="12" t="s">
+        <v>5969</v>
+      </c>
+      <c r="B1795" s="12" t="s">
+        <v>2906</v>
+      </c>
+      <c r="C1795" s="12" t="s">
         <v>5964</v>
       </c>
-      <c r="B1795" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1795" s="12" t="s">
+      <c r="D1795" s="12" t="s">
         <v>5965</v>
       </c>
-      <c r="D1795" s="12" t="s">
+      <c r="E1795" s="12" t="s">
         <v>5966</v>
-      </c>
-      <c r="E1795" s="12" t="s">
-        <v>5967</v>
       </c>
       <c r="F1795" s="12" t="s">
         <v>5953</v>
@@ -71820,10 +71820,10 @@
         <v>5959</v>
       </c>
       <c r="I1795" s="12" t="s">
+        <v>5967</v>
+      </c>
+      <c r="J1795" s="12" t="s">
         <v>5968</v>
-      </c>
-      <c r="J1795" s="12" t="s">
-        <v>5969</v>
       </c>
       <c r="K1795" s="12" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
optimize dql test case logic
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/btreecases/dql/casegroup1/sql_dql_cases1_btree.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/btreecases/dql/casegroup1/sql_dql_cases1_btree.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15594" uniqueCount="5970">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15568" uniqueCount="5970">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -21418,8 +21418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1795"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1765" workbookViewId="0">
-      <selection activeCell="C1798" sqref="C1798"/>
+    <sheetView tabSelected="1" topLeftCell="A970" workbookViewId="0">
+      <selection activeCell="G1573" sqref="G1573"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -21430,7 +21430,7 @@
     <col min="4" max="4" width="10.875" style="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.25" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="43.875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.875" style="1" customWidth="1"/>
     <col min="9" max="9" width="97.25" style="1" customWidth="1"/>
     <col min="10" max="10" width="30.125" style="1" customWidth="1"/>
@@ -64355,9 +64355,7 @@
       <c r="G1546" s="1" t="s">
         <v>2757</v>
       </c>
-      <c r="H1546" s="1" t="s">
-        <v>4942</v>
-      </c>
+      <c r="H1546" s="5"/>
       <c r="I1546" s="1" t="s">
         <v>2759</v>
       </c>
@@ -64390,9 +64388,7 @@
       <c r="G1547" s="1" t="s">
         <v>2758</v>
       </c>
-      <c r="H1547" s="1" t="s">
-        <v>4942</v>
-      </c>
+      <c r="H1547" s="5"/>
       <c r="I1547" s="1" t="s">
         <v>2760</v>
       </c>
@@ -64457,9 +64453,7 @@
       <c r="G1549" s="1" t="s">
         <v>2766</v>
       </c>
-      <c r="H1549" s="1" t="s">
-        <v>4945</v>
-      </c>
+      <c r="H1549" s="5"/>
       <c r="I1549" s="1" t="s">
         <v>2769</v>
       </c>
@@ -64492,9 +64486,7 @@
       <c r="G1550" s="1" t="s">
         <v>2767</v>
       </c>
-      <c r="H1550" s="1" t="s">
-        <v>4945</v>
-      </c>
+      <c r="H1550" s="5"/>
       <c r="I1550" s="1" t="s">
         <v>2770</v>
       </c>
@@ -64591,9 +64583,7 @@
       <c r="G1553" s="1" t="s">
         <v>2783</v>
       </c>
-      <c r="H1553" s="1" t="s">
-        <v>4949</v>
-      </c>
+      <c r="H1553" s="5"/>
       <c r="I1553" s="1" t="s">
         <v>2789</v>
       </c>
@@ -64626,9 +64616,7 @@
       <c r="G1554" s="1" t="s">
         <v>2784</v>
       </c>
-      <c r="H1554" s="1" t="s">
-        <v>4949</v>
-      </c>
+      <c r="H1554" s="5"/>
       <c r="I1554" s="1" t="s">
         <v>2790</v>
       </c>
@@ -64661,9 +64649,7 @@
       <c r="G1555" s="1" t="s">
         <v>2785</v>
       </c>
-      <c r="H1555" s="1" t="s">
-        <v>4949</v>
-      </c>
+      <c r="H1555" s="5"/>
       <c r="I1555" s="1" t="s">
         <v>2791</v>
       </c>
@@ -64696,9 +64682,7 @@
       <c r="G1556" s="1" t="s">
         <v>2786</v>
       </c>
-      <c r="H1556" s="1" t="s">
-        <v>4949</v>
-      </c>
+      <c r="H1556" s="5"/>
       <c r="I1556" s="1" t="s">
         <v>2792</v>
       </c>
@@ -64731,9 +64715,7 @@
       <c r="G1557" s="1" t="s">
         <v>2787</v>
       </c>
-      <c r="H1557" s="1" t="s">
-        <v>4949</v>
-      </c>
+      <c r="H1557" s="5"/>
       <c r="I1557" s="1" t="s">
         <v>2793</v>
       </c>
@@ -64798,9 +64780,7 @@
       <c r="G1559" s="1" t="s">
         <v>2797</v>
       </c>
-      <c r="H1559" s="1" t="s">
-        <v>4955</v>
-      </c>
+      <c r="H1559" s="5"/>
       <c r="I1559" s="1" t="s">
         <v>2801</v>
       </c>
@@ -64833,9 +64813,7 @@
       <c r="G1560" s="1" t="s">
         <v>2798</v>
       </c>
-      <c r="H1560" s="1" t="s">
-        <v>4955</v>
-      </c>
+      <c r="H1560" s="5"/>
       <c r="I1560" s="1" t="s">
         <v>2803</v>
       </c>
@@ -64868,9 +64846,7 @@
       <c r="G1561" s="1" t="s">
         <v>2799</v>
       </c>
-      <c r="H1561" s="1" t="s">
-        <v>4955</v>
-      </c>
+      <c r="H1561" s="5"/>
       <c r="I1561" s="1" t="s">
         <v>2804</v>
       </c>
@@ -64903,9 +64879,7 @@
       <c r="G1562" s="1" t="s">
         <v>2800</v>
       </c>
-      <c r="H1562" s="1" t="s">
-        <v>4955</v>
-      </c>
+      <c r="H1562" s="5"/>
       <c r="I1562" s="1" t="s">
         <v>2805</v>
       </c>
@@ -64970,9 +64944,7 @@
       <c r="G1564" s="1" t="s">
         <v>2809</v>
       </c>
-      <c r="H1564" s="1" t="s">
-        <v>4960</v>
-      </c>
+      <c r="H1564" s="5"/>
       <c r="I1564" s="1" t="s">
         <v>2812</v>
       </c>
@@ -65005,9 +64977,7 @@
       <c r="G1565" s="1" t="s">
         <v>2810</v>
       </c>
-      <c r="H1565" s="1" t="s">
-        <v>4960</v>
-      </c>
+      <c r="H1565" s="5"/>
       <c r="I1565" s="1" t="s">
         <v>2813</v>
       </c>
@@ -65072,9 +65042,7 @@
       <c r="G1567" s="1" t="s">
         <v>2816</v>
       </c>
-      <c r="H1567" s="1" t="s">
-        <v>4963</v>
-      </c>
+      <c r="H1567" s="5"/>
       <c r="I1567" s="1" t="s">
         <v>2819</v>
       </c>
@@ -65107,9 +65075,7 @@
       <c r="G1568" s="1" t="s">
         <v>2821</v>
       </c>
-      <c r="H1568" s="1" t="s">
-        <v>4949</v>
-      </c>
+      <c r="H1568" s="5"/>
       <c r="I1568" s="1" t="s">
         <v>2822</v>
       </c>
@@ -65142,9 +65108,7 @@
       <c r="G1569" s="1" t="s">
         <v>2831</v>
       </c>
-      <c r="H1569" s="1" t="s">
-        <v>4942</v>
-      </c>
+      <c r="H1569" s="5"/>
       <c r="I1569" s="1" t="s">
         <v>2830</v>
       </c>
@@ -65177,9 +65141,7 @@
       <c r="G1570" s="1" t="s">
         <v>2832</v>
       </c>
-      <c r="H1570" s="1" t="s">
-        <v>4945</v>
-      </c>
+      <c r="H1570" s="5"/>
       <c r="I1570" s="1" t="s">
         <v>2833</v>
       </c>
@@ -65212,9 +65174,7 @@
       <c r="G1571" s="1" t="s">
         <v>2834</v>
       </c>
-      <c r="H1571" s="1" t="s">
-        <v>4949</v>
-      </c>
+      <c r="H1571" s="5"/>
       <c r="I1571" s="1" t="s">
         <v>2835</v>
       </c>
@@ -65247,9 +65207,7 @@
       <c r="G1572" s="1" t="s">
         <v>2836</v>
       </c>
-      <c r="H1572" s="1" t="s">
-        <v>4948</v>
-      </c>
+      <c r="H1572" s="5"/>
       <c r="I1572" s="1" t="s">
         <v>2837</v>
       </c>
@@ -65282,9 +65240,7 @@
       <c r="G1573" s="1" t="s">
         <v>2838</v>
       </c>
-      <c r="H1573" s="1" t="s">
-        <v>4955</v>
-      </c>
+      <c r="H1573" s="5"/>
       <c r="I1573" s="1" t="s">
         <v>2839</v>
       </c>
@@ -65317,9 +65273,7 @@
       <c r="G1574" s="1" t="s">
         <v>2840</v>
       </c>
-      <c r="H1574" s="1" t="s">
-        <v>4960</v>
-      </c>
+      <c r="H1574" s="5"/>
       <c r="I1574" s="1" t="s">
         <v>2841</v>
       </c>
@@ -65352,9 +65306,7 @@
       <c r="G1575" s="1" t="s">
         <v>2842</v>
       </c>
-      <c r="H1575" s="1" t="s">
-        <v>4963</v>
-      </c>
+      <c r="H1575" s="5"/>
       <c r="I1575" s="1" t="s">
         <v>2843</v>
       </c>
@@ -65387,9 +65339,7 @@
       <c r="G1576" s="1" t="s">
         <v>2846</v>
       </c>
-      <c r="H1576" s="1" t="s">
-        <v>4942</v>
-      </c>
+      <c r="H1576" s="5"/>
       <c r="I1576" s="1" t="s">
         <v>2847</v>
       </c>
@@ -65422,9 +65372,7 @@
       <c r="G1577" s="1" t="s">
         <v>2848</v>
       </c>
-      <c r="H1577" s="1" t="s">
-        <v>4949</v>
-      </c>
+      <c r="H1577" s="5"/>
       <c r="I1577" s="1" t="s">
         <v>2849</v>
       </c>

</xml_diff>